<commit_message>
Added user in model 2
</commit_message>
<xml_diff>
--- a/Structure.xlsx
+++ b/Structure.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Naveed\Documents\Programming\Themes\QWheels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{428398EB-20C2-4116-8F0B-25FDD267CB30}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{E6F2AA8E-338B-4CCA-A6D4-08A28F51F5C4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{1BE5680A-B01C-40A4-9DA5-30409DCF74DF}"/>
   </bookViews>
@@ -16,6 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,7 +32,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+  <si>
+    <t>Product</t>
+  </si>
   <si>
     <t>Admin</t>
   </si>
@@ -106,6 +110,15 @@
   </si>
   <si>
     <t>Order History</t>
+  </si>
+  <si>
+    <t>Reviews</t>
+  </si>
+  <si>
+    <t>Images</t>
+  </si>
+  <si>
+    <t>Cart</t>
   </si>
 </sst>
 </file>
@@ -201,22 +214,22 @@
   <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -537,10 +550,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B845F106-3F1E-4097-806D-9641A0EBADBC}">
-  <dimension ref="A1:C21"/>
+  <dimension ref="A1:J21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -550,159 +563,171 @@
     <col min="3" max="3" width="16.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A2" s="9"/>
+      <c r="B2" s="6"/>
+      <c r="C2" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A3" s="9"/>
+      <c r="B3" s="6"/>
+      <c r="C3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H3" t="s">
+        <v>27</v>
+      </c>
+      <c r="I3" t="s">
+        <v>26</v>
+      </c>
+      <c r="J3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A4" s="9"/>
+      <c r="B4" s="6"/>
+      <c r="C4" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A5" s="9"/>
+      <c r="B5" s="6"/>
+      <c r="C5" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A6" s="9"/>
+      <c r="B6" s="6"/>
+      <c r="C6" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="9"/>
+      <c r="B7" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A8" s="9"/>
+      <c r="B8" s="7"/>
+      <c r="C8" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A9" s="9"/>
+      <c r="B9" s="7"/>
+      <c r="C9" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A10" s="9"/>
+      <c r="B10" s="7"/>
+      <c r="C10" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A11" s="9"/>
+      <c r="B11" s="7"/>
+      <c r="C11" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="4" t="s">
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A12" s="9"/>
+      <c r="B12" s="8" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A2" s="2"/>
-      <c r="B2" s="3"/>
-      <c r="C2" s="5" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A3" s="2"/>
-      <c r="B3" s="3"/>
-      <c r="C3" s="5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A4" s="2"/>
-      <c r="B4" s="3"/>
-      <c r="C4" s="6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A5" s="2"/>
-      <c r="B5" s="3"/>
-      <c r="C5" s="6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A6" s="2"/>
-      <c r="B6" s="3"/>
-      <c r="C6" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="2"/>
-      <c r="B7" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A8" s="2"/>
-      <c r="B8" s="7"/>
-      <c r="C8" s="5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A9" s="2"/>
-      <c r="B9" s="7"/>
-      <c r="C9" s="5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A10" s="2"/>
-      <c r="B10" s="7"/>
-      <c r="C10" s="6" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A11" s="2"/>
-      <c r="B11" s="7"/>
-      <c r="C11" s="6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A12" s="2"/>
-      <c r="B12" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="C12" s="5" t="s">
+      <c r="C12" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A13" s="9"/>
+      <c r="B13" s="8"/>
+      <c r="C13" s="3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A13" s="2"/>
-      <c r="B13" s="8"/>
-      <c r="C13" s="5" t="s">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A14" s="9"/>
+      <c r="B14" s="8"/>
+      <c r="C14" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A15" s="9"/>
+      <c r="B15" s="8"/>
+      <c r="C15" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A16" s="9"/>
+      <c r="B16" s="8"/>
+      <c r="C16" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A17" s="9"/>
+      <c r="B17" s="8"/>
+      <c r="C17" s="4" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A14" s="2"/>
-      <c r="B14" s="8"/>
-      <c r="C14" s="5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A15" s="2"/>
-      <c r="B15" s="8"/>
-      <c r="C15" s="5" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A16" s="2"/>
-      <c r="B16" s="8"/>
-      <c r="C16" s="6" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A17" s="2"/>
-      <c r="B17" s="8"/>
-      <c r="C17" s="6" t="s">
-        <v>16</v>
-      </c>
-    </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A18" s="2"/>
+      <c r="A18" s="9"/>
       <c r="B18" s="8"/>
-      <c r="C18" s="6" t="s">
-        <v>21</v>
+      <c r="C18" s="4" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A19" s="2"/>
+      <c r="A19" s="9"/>
       <c r="B19" s="8"/>
-      <c r="C19" s="9" t="s">
-        <v>22</v>
+      <c r="C19" s="5" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A20" s="2"/>
+      <c r="A20" s="9"/>
       <c r="B20" s="8"/>
-      <c r="C20" s="9" t="s">
+      <c r="C20" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A21" s="9"/>
+      <c r="B21" s="8"/>
+      <c r="C21" s="5" t="s">
         <v>24</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A21" s="2"/>
-      <c r="B21" s="8"/>
-      <c r="C21" s="9" t="s">
-        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>